<commit_message>
Adding something inside figure
</commit_message>
<xml_diff>
--- a/figure/fsperf.xlsx
+++ b/figure/fsperf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="008000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -314,7 +317,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF0000"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -370,11 +373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2092571784"/>
-        <c:axId val="2105089848"/>
+        <c:axId val="-2124329000"/>
+        <c:axId val="-2122527784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2092571784"/>
+        <c:axId val="-2124329000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,26 +390,26 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600">
+                  <a:defRPr sz="1200" b="0">
                     <a:latin typeface="Palatino"/>
                     <a:cs typeface="Palatino"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600">
+                  <a:rPr lang="en-US" sz="1200" b="0">
                     <a:latin typeface="Palatino"/>
                     <a:cs typeface="Palatino"/>
                   </a:rPr>
                   <a:t>Number</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0">
+                  <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
                     <a:latin typeface="Palatino"/>
                     <a:cs typeface="Palatino"/>
                   </a:rPr>
                   <a:t> of Threads</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1600">
+                <a:endParaRPr lang="en-US" sz="1200" b="0">
                   <a:latin typeface="Palatino"/>
                   <a:cs typeface="Palatino"/>
                 </a:endParaRPr>
@@ -433,7 +436,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2105089848"/>
+        <c:crossAx val="-2122527784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -441,7 +444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105089848"/>
+        <c:axId val="-2122527784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -455,13 +458,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600">
+                  <a:defRPr sz="1200">
                     <a:latin typeface="Palatino"/>
                     <a:cs typeface="Palatino"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600">
+                  <a:rPr lang="en-US" sz="1200">
                     <a:latin typeface="Palatino"/>
                     <a:cs typeface="Palatino"/>
                   </a:rPr>
@@ -490,7 +493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2092571784"/>
+        <c:crossAx val="-2124329000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -513,7 +516,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="1">
+            <a:defRPr sz="1200" b="0">
               <a:latin typeface="Palatino"/>
               <a:cs typeface="Palatino"/>
             </a:defRPr>
@@ -859,11 +862,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2092250872"/>
-        <c:axId val="2092714728"/>
+        <c:axId val="-2122768296"/>
+        <c:axId val="-2122765288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2092250872"/>
+        <c:axId val="-2122768296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2092714728"/>
+        <c:crossAx val="-2122765288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -890,7 +893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092714728"/>
+        <c:axId val="-2122765288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092250872"/>
+        <c:crossAx val="-2122768296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.02"/>
@@ -1110,11 +1113,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2103124712"/>
-        <c:axId val="2103331640"/>
+        <c:axId val="-2123037480"/>
+        <c:axId val="-2123034536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2103124712"/>
+        <c:axId val="-2123037480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1123,7 +1126,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103331640"/>
+        <c:crossAx val="-2123034536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1131,7 +1134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103331640"/>
+        <c:axId val="-2123034536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,14 +1162,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103124712"/>
+        <c:crossAx val="-2123037480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.001"/>
@@ -1622,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1703,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>